<commit_message>
corrects missing min/max values and project coverage
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_catch_metadata.xlsx
+++ b/data-raw/metadata/camp_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59311B23-996A-7543-8196-34665BBD7F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BC909-E650-2A47-A6B7-DD6D3AD45AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-12120" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="275">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -846,12 +846,18 @@
   <si>
     <t>2022-05-18 02:30:56</t>
   </si>
+  <si>
+    <t>2006-10-02 09:30:00</t>
+  </si>
+  <si>
+    <t>2022-05-18 09:30:56 UTC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -874,6 +880,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -915,7 +927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -938,9 +950,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,7 +1173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1983,10 +1996,10 @@
         <v>62</v>
       </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="12" t="s">
+      <c r="L20" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="M20" s="10" t="s">
         <v>272</v>
       </c>
       <c r="N20" s="4"/>
@@ -2027,8 +2040,12 @@
         <v>62</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -2270,7 +2287,7 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
@@ -2298,7 +2315,7 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
@@ -2326,7 +2343,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
@@ -2354,7 +2371,7 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>

</xml_diff>

<commit_message>
fixes mispelling in catch metadata table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_catch_metadata.xlsx
+++ b/data-raw/metadata/camp_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BC909-E650-2A47-A6B7-DD6D3AD45AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69521F-C114-A845-B380-3F27EAB30ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="274">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Total length of the fish measured in millimeters</t>
-  </si>
-  <si>
-    <t>catcg</t>
   </si>
   <si>
     <t>weight</t>
@@ -850,7 +847,7 @@
     <t>2006-10-02 09:30:00</t>
   </si>
   <si>
-    <t>2022-05-18 09:30:56 UTC</t>
+    <t>2022-05-18 09:30:56</t>
   </si>
 </sst>
 </file>
@@ -868,17 +865,20 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -951,9 +951,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,7 +1173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1686,7 +1686,7 @@
         <v>42</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>44</v>
@@ -1725,7 +1725,7 @@
         <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>43</v>
@@ -1734,7 +1734,7 @@
         <v>42</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>44</v>
@@ -1764,10 +1764,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>42</v>
@@ -1782,7 +1782,7 @@
         <v>42</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>44</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>42</v>
@@ -1830,10 +1830,10 @@
         <v>42</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
@@ -1860,10 +1860,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1936,10 +1936,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1974,33 +1974,33 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
       <c r="J20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="M20" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2018,33 +2018,33 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
       <c r="J21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="M21" s="10" t="s">
         <v>273</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
@@ -2287,7 +2287,7 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
@@ -2315,7 +2315,7 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
@@ -2343,7 +2343,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
@@ -2371,7 +2371,7 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
@@ -29306,7 +29306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A98" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -29320,13 +29320,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -29357,7 +29357,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>13</v>
@@ -29391,7 +29391,7 @@
         <v>159697</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>26</v>
@@ -29425,7 +29425,7 @@
         <v>159698</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>26</v>
@@ -29459,7 +29459,7 @@
         <v>159700</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>26</v>
@@ -29493,7 +29493,7 @@
         <v>159707</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>26</v>
@@ -29527,7 +29527,7 @@
         <v>159709</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>26</v>
@@ -29561,7 +29561,7 @@
         <v>159710</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>26</v>
@@ -29595,7 +29595,7 @@
         <v>159713</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>26</v>
@@ -29629,7 +29629,7 @@
         <v>161030</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>26</v>
@@ -29663,7 +29663,7 @@
         <v>161064</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>26</v>
@@ -29697,7 +29697,7 @@
         <v>161067</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>26</v>
@@ -29731,7 +29731,7 @@
         <v>161068</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>26</v>
@@ -29765,7 +29765,7 @@
         <v>161127</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>26</v>
@@ -29799,7 +29799,7 @@
         <v>161702</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>26</v>
@@ -29833,7 +29833,7 @@
         <v>161738</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>26</v>
@@ -29867,7 +29867,7 @@
         <v>161931</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>26</v>
@@ -29901,7 +29901,7 @@
         <v>161974</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>26</v>
@@ -29935,7 +29935,7 @@
         <v>161975</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>26</v>
@@ -29969,7 +29969,7 @@
         <v>161977</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>26</v>
@@ -30003,7 +30003,7 @@
         <v>161979</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>26</v>
@@ -30037,7 +30037,7 @@
         <v>161980</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>26</v>
@@ -30071,7 +30071,7 @@
         <v>161989</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>26</v>
@@ -30105,7 +30105,7 @@
         <v>161997</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>26</v>
@@ -30139,7 +30139,7 @@
         <v>162003</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>26</v>
@@ -30173,7 +30173,7 @@
         <v>162032</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>26</v>
@@ -30207,7 +30207,7 @@
         <v>162033</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>26</v>
@@ -30241,7 +30241,7 @@
         <v>163342</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>26</v>
@@ -30275,7 +30275,7 @@
         <v>163344</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>26</v>
@@ -30309,7 +30309,7 @@
         <v>163350</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>26</v>
@@ -30343,7 +30343,7 @@
         <v>163368</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>26</v>
@@ -30377,7 +30377,7 @@
         <v>163387</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>26</v>
@@ -30411,7 +30411,7 @@
         <v>163517</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>26</v>
@@ -30445,7 +30445,7 @@
         <v>163524</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>26</v>
@@ -30479,7 +30479,7 @@
         <v>163565</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>26</v>
@@ -30513,7 +30513,7 @@
         <v>163569</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>26</v>
@@ -30547,7 +30547,7 @@
         <v>163587</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>26</v>
@@ -30581,7 +30581,7 @@
         <v>163589</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>26</v>
@@ -30615,7 +30615,7 @@
         <v>163603</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>26</v>
@@ -30649,7 +30649,7 @@
         <v>163792</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>26</v>
@@ -30683,7 +30683,7 @@
         <v>163892</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>26</v>
@@ -30717,7 +30717,7 @@
         <v>163908</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>26</v>
@@ -30751,7 +30751,7 @@
         <v>163995</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>26</v>
@@ -30785,7 +30785,7 @@
         <v>163998</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>26</v>
@@ -30819,7 +30819,7 @@
         <v>164034</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>26</v>
@@ -30853,7 +30853,7 @@
         <v>164037</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
@@ -30887,7 +30887,7 @@
         <v>164039</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
@@ -30921,7 +30921,7 @@
         <v>164041</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>26</v>
@@ -30955,7 +30955,7 @@
         <v>164043</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>26</v>
@@ -30989,7 +30989,7 @@
         <v>165679</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>26</v>
@@ -31023,7 +31023,7 @@
         <v>165877</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>26</v>
@@ -31057,7 +31057,7 @@
         <v>165878</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>26</v>
@@ -31091,7 +31091,7 @@
         <v>165993</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>26</v>
@@ -31125,7 +31125,7 @@
         <v>165998</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>26</v>
@@ -31159,7 +31159,7 @@
         <v>166365</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>26</v>
@@ -31193,7 +31193,7 @@
         <v>167229</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>26</v>
@@ -31227,7 +31227,7 @@
         <v>167233</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>26</v>
@@ -31261,7 +31261,7 @@
         <v>167234</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>26</v>
@@ -31295,7 +31295,7 @@
         <v>167680</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>26</v>
@@ -31329,7 +31329,7 @@
         <v>168093</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>26</v>
@@ -31363,7 +31363,7 @@
         <v>168130</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>26</v>
@@ -31397,7 +31397,7 @@
         <v>168132</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>26</v>
@@ -31431,7 +31431,7 @@
         <v>168139</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>26</v>
@@ -31465,7 +31465,7 @@
         <v>168141</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>26</v>
@@ -31499,7 +31499,7 @@
         <v>168144</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>26</v>
@@ -31533,7 +31533,7 @@
         <v>168154</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>26</v>
@@ -31567,7 +31567,7 @@
         <v>168158</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>26</v>
@@ -31601,7 +31601,7 @@
         <v>168160</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>26</v>
@@ -31635,7 +31635,7 @@
         <v>168161</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>26</v>
@@ -31669,7 +31669,7 @@
         <v>168163</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>26</v>
@@ -31703,7 +31703,7 @@
         <v>168165</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>26</v>
@@ -31737,7 +31737,7 @@
         <v>168166</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>26</v>
@@ -31771,7 +31771,7 @@
         <v>168167</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>26</v>
@@ -31805,7 +31805,7 @@
         <v>168175</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>26</v>
@@ -31839,7 +31839,7 @@
         <v>168487</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>26</v>
@@ -31873,7 +31873,7 @@
         <v>171882</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>26</v>
@@ -31907,7 +31907,7 @@
         <v>250</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>26</v>
@@ -31941,7 +31941,7 @@
         <v>251</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>26</v>
@@ -31975,7 +31975,7 @@
         <v>252</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>26</v>
@@ -32009,7 +32009,7 @@
         <v>253</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>26</v>
@@ -32043,7 +32043,7 @@
         <v>254</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>26</v>
@@ -32077,7 +32077,7 @@
         <v>255</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>26</v>
@@ -32111,7 +32111,7 @@
         <v>550562</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>26</v>
@@ -32145,7 +32145,7 @@
         <v>553322</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>26</v>
@@ -32179,7 +32179,7 @@
         <v>622248</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>26</v>
@@ -32213,7 +32213,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>28</v>
@@ -32247,7 +32247,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>28</v>
@@ -32281,7 +32281,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>28</v>
@@ -32315,7 +32315,7 @@
         <v>252</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>28</v>
@@ -32349,7 +32349,7 @@
         <v>251</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>28</v>
@@ -32383,7 +32383,7 @@
         <v>255</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>28</v>
@@ -32417,7 +32417,7 @@
         <v>250</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>28</v>
@@ -32451,7 +32451,7 @@
         <v>254</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>28</v>
@@ -32485,7 +32485,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>28</v>
@@ -32519,7 +32519,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>28</v>
@@ -32553,7 +32553,7 @@
         <v>253</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>28</v>
@@ -32587,7 +32587,7 @@
         <v>4</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>28</v>
@@ -32621,7 +32621,7 @@
         <v>3</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>32</v>
@@ -32655,7 +32655,7 @@
         <v>5</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>32</v>
@@ -32689,7 +32689,7 @@
         <v>6</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>32</v>
@@ -32723,7 +32723,7 @@
         <v>252</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>32</v>
@@ -32757,7 +32757,7 @@
         <v>251</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>32</v>
@@ -32791,7 +32791,7 @@
         <v>255</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>32</v>
@@ -32825,7 +32825,7 @@
         <v>250</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>32</v>
@@ -32859,7 +32859,7 @@
         <v>254</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>32</v>
@@ -32893,7 +32893,7 @@
         <v>1</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>32</v>
@@ -32927,7 +32927,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>32</v>
@@ -32961,7 +32961,7 @@
         <v>253</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>32</v>
@@ -32995,7 +32995,7 @@
         <v>4</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>32</v>
@@ -33029,7 +33029,7 @@
         <v>5</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>30</v>
@@ -33063,7 +33063,7 @@
         <v>3</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>30</v>
@@ -33097,7 +33097,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>30</v>
@@ -33131,7 +33131,7 @@
         <v>6</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>30</v>
@@ -33165,7 +33165,7 @@
         <v>4</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>30</v>
@@ -33199,7 +33199,7 @@
         <v>252</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>30</v>
@@ -33233,7 +33233,7 @@
         <v>251</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>30</v>
@@ -33267,7 +33267,7 @@
         <v>255</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>30</v>
@@ -33301,7 +33301,7 @@
         <v>1</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>30</v>
@@ -33335,7 +33335,7 @@
         <v>250</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>30</v>
@@ -33369,7 +33369,7 @@
         <v>254</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>30</v>
@@ -33403,7 +33403,7 @@
         <v>253</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>30</v>
@@ -33437,7 +33437,7 @@
         <v>5</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>34</v>
@@ -33471,7 +33471,7 @@
         <v>3</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>34</v>
@@ -33505,7 +33505,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>34</v>
@@ -33539,7 +33539,7 @@
         <v>6</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>34</v>
@@ -33573,7 +33573,7 @@
         <v>4</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>34</v>
@@ -33607,7 +33607,7 @@
         <v>252</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>34</v>
@@ -33641,7 +33641,7 @@
         <v>251</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>34</v>
@@ -33675,7 +33675,7 @@
         <v>255</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>34</v>
@@ -33709,7 +33709,7 @@
         <v>1</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>34</v>
@@ -33743,7 +33743,7 @@
         <v>250</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>34</v>
@@ -33777,7 +33777,7 @@
         <v>254</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>34</v>
@@ -33811,7 +33811,7 @@
         <v>253</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>34</v>
@@ -33845,7 +33845,7 @@
         <v>1</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>36</v>
@@ -33879,7 +33879,7 @@
         <v>3</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>36</v>
@@ -33913,7 +33913,7 @@
         <v>2</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>36</v>
@@ -33947,7 +33947,7 @@
         <v>252</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>36</v>
@@ -33981,7 +33981,7 @@
         <v>251</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>36</v>
@@ -34015,7 +34015,7 @@
         <v>255</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>36</v>
@@ -34049,7 +34049,7 @@
         <v>250</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>36</v>
@@ -34083,7 +34083,7 @@
         <v>254</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C141" s="8" t="s">
         <v>36</v>
@@ -34117,7 +34117,7 @@
         <v>253</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>36</v>
@@ -34151,7 +34151,7 @@
         <v>11</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>38</v>
@@ -34185,7 +34185,7 @@
         <v>6</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C144" s="8" t="s">
         <v>38</v>
@@ -34219,7 +34219,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C145" s="8" t="s">
         <v>38</v>
@@ -34253,7 +34253,7 @@
         <v>17</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C146" s="8" t="s">
         <v>38</v>
@@ -34287,7 +34287,7 @@
         <v>3</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C147" s="8" t="s">
         <v>38</v>
@@ -34321,7 +34321,7 @@
         <v>15</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C148" s="8" t="s">
         <v>38</v>
@@ -34355,7 +34355,7 @@
         <v>10</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C149" s="8" t="s">
         <v>38</v>
@@ -34389,7 +34389,7 @@
         <v>16</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C150" s="8" t="s">
         <v>38</v>
@@ -34423,7 +34423,7 @@
         <v>13</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>38</v>
@@ -34457,7 +34457,7 @@
         <v>14</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C152" s="8" t="s">
         <v>38</v>
@@ -34491,7 +34491,7 @@
         <v>252</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C153" s="8" t="s">
         <v>38</v>
@@ -34525,7 +34525,7 @@
         <v>251</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C154" s="8" t="s">
         <v>38</v>
@@ -34559,7 +34559,7 @@
         <v>255</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C155" s="8" t="s">
         <v>38</v>
@@ -34593,7 +34593,7 @@
         <v>250</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C156" s="8" t="s">
         <v>38</v>
@@ -34627,7 +34627,7 @@
         <v>4</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C157" s="8" t="s">
         <v>38</v>
@@ -34661,7 +34661,7 @@
         <v>7</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>38</v>
@@ -34695,7 +34695,7 @@
         <v>19</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>38</v>
@@ -34729,7 +34729,7 @@
         <v>254</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>38</v>
@@ -34763,7 +34763,7 @@
         <v>5</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>38</v>
@@ -34797,7 +34797,7 @@
         <v>8</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>38</v>
@@ -34831,7 +34831,7 @@
         <v>20</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C163" s="8" t="s">
         <v>38</v>
@@ -34865,7 +34865,7 @@
         <v>18</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C164" s="8" t="s">
         <v>38</v>
@@ -34899,7 +34899,7 @@
         <v>253</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C165" s="8" t="s">
         <v>38</v>
@@ -34933,7 +34933,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>38</v>
@@ -34967,7 +34967,7 @@
         <v>1</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C167" s="8" t="s">
         <v>38</v>
@@ -35001,7 +35001,7 @@
         <v>2</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C168" s="8" t="s">
         <v>38</v>
@@ -35035,10 +35035,10 @@
         <v>2</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D169" s="9"/>
       <c r="E169" s="9"/>
@@ -35069,10 +35069,10 @@
         <v>252</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D170" s="9"/>
       <c r="E170" s="9"/>
@@ -35103,10 +35103,10 @@
         <v>251</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D171" s="9"/>
       <c r="E171" s="9"/>
@@ -35137,10 +35137,10 @@
         <v>255</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D172" s="9"/>
       <c r="E172" s="9"/>
@@ -35171,10 +35171,10 @@
         <v>250</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D173" s="9"/>
       <c r="E173" s="9"/>
@@ -35205,10 +35205,10 @@
         <v>254</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
@@ -35239,10 +35239,10 @@
         <v>253</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D175" s="9"/>
       <c r="E175" s="9"/>
@@ -35273,10 +35273,10 @@
         <v>1</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D176" s="9"/>
       <c r="E176" s="9"/>
@@ -35307,10 +35307,10 @@
         <v>2</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D177" s="9"/>
       <c r="E177" s="9"/>
@@ -35341,10 +35341,10 @@
         <v>252</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D178" s="9"/>
       <c r="E178" s="9"/>
@@ -35375,10 +35375,10 @@
         <v>251</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D179" s="9"/>
       <c r="E179" s="9"/>
@@ -35409,10 +35409,10 @@
         <v>255</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D180" s="9"/>
       <c r="E180" s="9"/>
@@ -35443,10 +35443,10 @@
         <v>250</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D181" s="9"/>
       <c r="E181" s="9"/>
@@ -35477,10 +35477,10 @@
         <v>254</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D182" s="9"/>
       <c r="E182" s="9"/>
@@ -35511,10 +35511,10 @@
         <v>253</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D183" s="9"/>
       <c r="E183" s="9"/>
@@ -35545,10 +35545,10 @@
         <v>1</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D184" s="9"/>
       <c r="E184" s="9"/>
@@ -35579,10 +35579,10 @@
         <v>2</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D185" s="9"/>
       <c r="E185" s="9"/>
@@ -35613,10 +35613,10 @@
         <v>252</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D186" s="9"/>
       <c r="E186" s="9"/>
@@ -35647,10 +35647,10 @@
         <v>251</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D187" s="9"/>
       <c r="E187" s="9"/>
@@ -35681,10 +35681,10 @@
         <v>255</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D188" s="9"/>
       <c r="E188" s="9"/>
@@ -35715,10 +35715,10 @@
         <v>250</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D189" s="9"/>
       <c r="E189" s="9"/>
@@ -35749,10 +35749,10 @@
         <v>254</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D190" s="9"/>
       <c r="E190" s="9"/>
@@ -35783,10 +35783,10 @@
         <v>253</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D191" s="9"/>
       <c r="E191" s="9"/>
@@ -35817,10 +35817,10 @@
         <v>1</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D192" s="9"/>
       <c r="E192" s="9"/>
@@ -35851,10 +35851,10 @@
         <v>2</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D193" s="9"/>
       <c r="E193" s="9"/>
@@ -35885,10 +35885,10 @@
         <v>5</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D194" s="9"/>
       <c r="E194" s="9"/>
@@ -35919,10 +35919,10 @@
         <v>4</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D195" s="9"/>
       <c r="E195" s="9"/>
@@ -35953,10 +35953,10 @@
         <v>252</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="9"/>
@@ -35987,10 +35987,10 @@
         <v>251</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D197" s="9"/>
       <c r="E197" s="9"/>
@@ -36021,10 +36021,10 @@
         <v>255</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D198" s="9"/>
       <c r="E198" s="9"/>
@@ -36055,10 +36055,10 @@
         <v>250</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D199" s="9"/>
       <c r="E199" s="9"/>
@@ -36089,10 +36089,10 @@
         <v>254</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D200" s="9"/>
       <c r="E200" s="9"/>
@@ -36123,10 +36123,10 @@
         <v>6</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D201" s="9"/>
       <c r="E201" s="9"/>
@@ -36157,10 +36157,10 @@
         <v>1</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D202" s="9"/>
       <c r="E202" s="9"/>
@@ -36191,10 +36191,10 @@
         <v>253</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D203" s="9"/>
       <c r="E203" s="9"/>
@@ -36225,10 +36225,10 @@
         <v>3</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D204" s="9"/>
       <c r="E204" s="9"/>
@@ -36259,10 +36259,10 @@
         <v>3000</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D205" s="9"/>
       <c r="E205" s="9"/>
@@ -36293,10 +36293,10 @@
         <v>44000</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D206" s="9"/>
       <c r="E206" s="9"/>
@@ -36327,10 +36327,10 @@
         <v>52000</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D207" s="9"/>
       <c r="E207" s="9"/>
@@ -36361,10 +36361,10 @@
         <v>51000</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D208" s="9"/>
       <c r="E208" s="9"/>
@@ -36395,10 +36395,10 @@
         <v>5000</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="9"/>
@@ -36429,10 +36429,10 @@
         <v>46000</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D210" s="9"/>
       <c r="E210" s="9"/>
@@ -36463,10 +36463,10 @@
         <v>4000</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D211" s="9"/>
       <c r="E211" s="9"/>
@@ -36497,10 +36497,10 @@
         <v>45000</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D212" s="9"/>
       <c r="E212" s="9"/>
@@ -36531,10 +36531,10 @@
         <v>252</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D213" s="9"/>
       <c r="E213" s="9"/>
@@ -36565,10 +36565,10 @@
         <v>251</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D214" s="9"/>
       <c r="E214" s="9"/>
@@ -36599,10 +36599,10 @@
         <v>255</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D215" s="9"/>
       <c r="E215" s="9"/>
@@ -36633,10 +36633,10 @@
         <v>53000</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D216" s="9"/>
       <c r="E216" s="9"/>
@@ -36667,10 +36667,10 @@
         <v>54000</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D217" s="9"/>
       <c r="E217" s="9"/>
@@ -36701,10 +36701,10 @@
         <v>55000</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D218" s="9"/>
       <c r="E218" s="9"/>
@@ -36735,10 +36735,10 @@
         <v>56000</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D219" s="9"/>
       <c r="E219" s="9"/>
@@ -36769,10 +36769,10 @@
         <v>50000</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D220" s="9"/>
       <c r="E220" s="9"/>
@@ -36803,10 +36803,10 @@
         <v>7000</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D221" s="9"/>
       <c r="E221" s="9"/>
@@ -36837,10 +36837,10 @@
         <v>2000</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D222" s="9"/>
       <c r="E222" s="9"/>
@@ -36871,10 +36871,10 @@
         <v>43000</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D223" s="9"/>
       <c r="E223" s="9"/>
@@ -36905,10 +36905,10 @@
         <v>6000</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D224" s="9"/>
       <c r="E224" s="9"/>
@@ -36939,10 +36939,10 @@
         <v>47000</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D225" s="9"/>
       <c r="E225" s="9"/>
@@ -36973,10 +36973,10 @@
         <v>90000</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D226" s="9"/>
       <c r="E226" s="9"/>
@@ -37007,10 +37007,10 @@
         <v>253</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D227" s="9"/>
       <c r="E227" s="9"/>
@@ -37041,10 +37041,10 @@
         <v>2001</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D228" s="9"/>
       <c r="E228" s="9"/>
@@ -37075,10 +37075,10 @@
         <v>44018</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D229" s="9"/>
       <c r="E229" s="9"/>
@@ -37109,10 +37109,10 @@
         <v>44007</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D230" s="9"/>
       <c r="E230" s="9"/>
@@ -37143,10 +37143,10 @@
         <v>44017</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D231" s="9"/>
       <c r="E231" s="9"/>
@@ -37177,10 +37177,10 @@
         <v>44016</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D232" s="9"/>
       <c r="E232" s="9"/>
@@ -37211,10 +37211,10 @@
         <v>44013</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D233" s="9"/>
       <c r="E233" s="9"/>
@@ -37245,10 +37245,10 @@
         <v>3001</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C234" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D234" s="9"/>
       <c r="E234" s="9"/>
@@ -37279,10 +37279,10 @@
         <v>3002</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C235" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D235" s="9"/>
       <c r="E235" s="9"/>
@@ -37313,10 +37313,10 @@
         <v>52003</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C236" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D236" s="9"/>
       <c r="E236" s="9"/>
@@ -37347,10 +37347,10 @@
         <v>51002</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D237" s="9"/>
       <c r="E237" s="9"/>
@@ -37381,10 +37381,10 @@
         <v>51003</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D238" s="9"/>
       <c r="E238" s="9"/>
@@ -37415,10 +37415,10 @@
         <v>52001</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D239" s="9"/>
       <c r="E239" s="9"/>
@@ -37449,10 +37449,10 @@
         <v>52002</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D240" s="9"/>
       <c r="E240" s="9"/>
@@ -37483,10 +37483,10 @@
         <v>52004</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D241" s="9"/>
       <c r="E241" s="9"/>
@@ -37517,10 +37517,10 @@
         <v>90001</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C242" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D242" s="9"/>
       <c r="E242" s="9"/>
@@ -37551,10 +37551,10 @@
         <v>46003</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D243" s="9"/>
       <c r="E243" s="9"/>
@@ -37585,10 +37585,10 @@
         <v>46001</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D244" s="9"/>
       <c r="E244" s="9"/>
@@ -37619,10 +37619,10 @@
         <v>46004</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D245" s="9"/>
       <c r="E245" s="9"/>
@@ -37653,10 +37653,10 @@
         <v>5001</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C246" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D246" s="9"/>
       <c r="E246" s="9"/>
@@ -37687,10 +37687,10 @@
         <v>5003</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D247" s="9"/>
       <c r="E247" s="9"/>
@@ -37721,10 +37721,10 @@
         <v>5002</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C248" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D248" s="9"/>
       <c r="E248" s="9"/>
@@ -37755,10 +37755,10 @@
         <v>4001</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D249" s="9"/>
       <c r="E249" s="9"/>
@@ -37789,10 +37789,10 @@
         <v>4002</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C250" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D250" s="9"/>
       <c r="E250" s="9"/>
@@ -37823,10 +37823,10 @@
         <v>44010</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D251" s="9"/>
       <c r="E251" s="9"/>
@@ -37857,10 +37857,10 @@
         <v>51001</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D252" s="9"/>
       <c r="E252" s="9"/>
@@ -37891,10 +37891,10 @@
         <v>46002</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D253" s="9"/>
       <c r="E253" s="9"/>
@@ -37925,10 +37925,10 @@
         <v>43000</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D254" s="9"/>
       <c r="E254" s="9"/>
@@ -37959,10 +37959,10 @@
         <v>44000</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D255" s="9"/>
       <c r="E255" s="9"/>
@@ -37993,10 +37993,10 @@
         <v>45000</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D256" s="9"/>
       <c r="E256" s="9"/>
@@ -38027,10 +38027,10 @@
         <v>46000</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D257" s="9"/>
       <c r="E257" s="9"/>
@@ -38061,10 +38061,10 @@
         <v>47000</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D258" s="9"/>
       <c r="E258" s="9"/>
@@ -38095,10 +38095,10 @@
         <v>50000</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D259" s="9"/>
       <c r="E259" s="9"/>
@@ -38129,10 +38129,10 @@
         <v>51000</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D260" s="9"/>
       <c r="E260" s="9"/>
@@ -38163,10 +38163,10 @@
         <v>52000</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D261" s="9"/>
       <c r="E261" s="9"/>
@@ -38197,10 +38197,10 @@
         <v>53000</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D262" s="9"/>
       <c r="E262" s="9"/>
@@ -38231,10 +38231,10 @@
         <v>54000</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D263" s="9"/>
       <c r="E263" s="9"/>
@@ -38265,10 +38265,10 @@
         <v>55000</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D264" s="9"/>
       <c r="E264" s="9"/>
@@ -38299,10 +38299,10 @@
         <v>56000</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D265" s="9"/>
       <c r="E265" s="9"/>
@@ -38333,10 +38333,10 @@
         <v>90000</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D266" s="9"/>
       <c r="E266" s="9"/>
@@ -38367,10 +38367,10 @@
         <v>44001</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D267" s="9"/>
       <c r="E267" s="9"/>
@@ -38401,10 +38401,10 @@
         <v>44003</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D268" s="9"/>
       <c r="E268" s="9"/>
@@ -38435,10 +38435,10 @@
         <v>44002</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D269" s="9"/>
       <c r="E269" s="9"/>
@@ -38469,10 +38469,10 @@
         <v>44004</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D270" s="9"/>
       <c r="E270" s="9"/>
@@ -38503,10 +38503,10 @@
         <v>47002</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D271" s="9"/>
       <c r="E271" s="9"/>
@@ -38537,10 +38537,10 @@
         <v>47001</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D272" s="9"/>
       <c r="E272" s="9"/>
@@ -38571,10 +38571,10 @@
         <v>44009</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D273" s="9"/>
       <c r="E273" s="9"/>
@@ -38605,10 +38605,10 @@
         <v>44006</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D274" s="9"/>
       <c r="E274" s="9"/>
@@ -38639,10 +38639,10 @@
         <v>44008</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D275" s="9"/>
       <c r="E275" s="9"/>
@@ -38673,10 +38673,10 @@
         <v>7002</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D276" s="9"/>
       <c r="E276" s="9"/>
@@ -38707,10 +38707,10 @@
         <v>7003</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D277" s="9"/>
       <c r="E277" s="9"/>
@@ -38741,10 +38741,10 @@
         <v>44012</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D278" s="9"/>
       <c r="E278" s="9"/>
@@ -38775,10 +38775,10 @@
         <v>44014</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D279" s="9"/>
       <c r="E279" s="9"/>
@@ -38809,10 +38809,10 @@
         <v>44011</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D280" s="9"/>
       <c r="E280" s="9"/>
@@ -38843,10 +38843,10 @@
         <v>44015</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D281" s="9"/>
       <c r="E281" s="9"/>
@@ -38877,10 +38877,10 @@
         <v>44005</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D282" s="9"/>
       <c r="E282" s="9"/>
@@ -38911,10 +38911,10 @@
         <v>43001</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D283" s="9"/>
       <c r="E283" s="9"/>
@@ -38945,10 +38945,10 @@
         <v>2004</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D284" s="9"/>
       <c r="E284" s="9"/>
@@ -38979,10 +38979,10 @@
         <v>2003</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D285" s="9"/>
       <c r="E285" s="9"/>
@@ -39013,10 +39013,10 @@
         <v>2002</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D286" s="9"/>
       <c r="E286" s="9"/>
@@ -39047,10 +39047,10 @@
         <v>2005</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D287" s="9"/>
       <c r="E287" s="9"/>
@@ -39081,10 +39081,10 @@
         <v>6002</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D288" s="9"/>
       <c r="E288" s="9"/>
@@ -39115,10 +39115,10 @@
         <v>6003</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D289" s="9"/>
       <c r="E289" s="9"/>

</xml_diff>

<commit_message>
updates project description ID to right value
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_catch_metadata.xlsx
+++ b/data-raw/metadata/camp_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69521F-C114-A845-B380-3F27EAB30ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA45FA-579C-8449-AD52-EAA750699473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>attribute_name</t>
-  </si>
-  <si>
-    <t>Feather River RST Program</t>
   </si>
   <si>
     <t>Unknown lamprey (Entosphenus or Lampetra)</t>
@@ -849,6 +846,9 @@
   <si>
     <t>2022-05-18 09:30:56</t>
   </si>
+  <si>
+    <t>Knights Landing RST program</t>
+  </si>
 </sst>
 </file>
 
@@ -1171,7 +1171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
@@ -1686,7 +1686,7 @@
         <v>42</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>44</v>
@@ -1734,7 +1734,7 @@
         <v>42</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>44</v>
@@ -1782,7 +1782,7 @@
         <v>42</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>44</v>
@@ -1830,7 +1830,7 @@
         <v>42</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>51</v>
@@ -1997,10 +1997,10 @@
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="M20" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>271</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2041,10 +2041,10 @@
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="M21" s="10" t="s">
         <v>272</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>273</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -29306,8 +29306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29354,10 +29354,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>73</v>
+        <v>273</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>13</v>
@@ -29391,7 +29391,7 @@
         <v>159697</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>26</v>
@@ -29425,7 +29425,7 @@
         <v>159698</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>26</v>
@@ -29459,7 +29459,7 @@
         <v>159700</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>26</v>
@@ -29493,7 +29493,7 @@
         <v>159707</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>26</v>
@@ -29527,7 +29527,7 @@
         <v>159709</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>26</v>
@@ -29561,7 +29561,7 @@
         <v>159710</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>26</v>
@@ -29595,7 +29595,7 @@
         <v>159713</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>26</v>
@@ -29629,7 +29629,7 @@
         <v>161030</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>26</v>
@@ -29663,7 +29663,7 @@
         <v>161064</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>26</v>
@@ -29697,7 +29697,7 @@
         <v>161067</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>26</v>
@@ -29731,7 +29731,7 @@
         <v>161068</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>26</v>
@@ -29765,7 +29765,7 @@
         <v>161127</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>26</v>
@@ -29799,7 +29799,7 @@
         <v>161702</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>26</v>
@@ -29833,7 +29833,7 @@
         <v>161738</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>26</v>
@@ -29867,7 +29867,7 @@
         <v>161931</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>26</v>
@@ -29901,7 +29901,7 @@
         <v>161974</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>26</v>
@@ -29935,7 +29935,7 @@
         <v>161975</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>26</v>
@@ -29969,7 +29969,7 @@
         <v>161977</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>26</v>
@@ -30003,7 +30003,7 @@
         <v>161979</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>26</v>
@@ -30037,7 +30037,7 @@
         <v>161980</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>26</v>
@@ -30071,7 +30071,7 @@
         <v>161989</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>26</v>
@@ -30105,7 +30105,7 @@
         <v>161997</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>26</v>
@@ -30139,7 +30139,7 @@
         <v>162003</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>26</v>
@@ -30173,7 +30173,7 @@
         <v>162032</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>26</v>
@@ -30207,7 +30207,7 @@
         <v>162033</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>26</v>
@@ -30241,7 +30241,7 @@
         <v>163342</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>26</v>
@@ -30275,7 +30275,7 @@
         <v>163344</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>26</v>
@@ -30309,7 +30309,7 @@
         <v>163350</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>26</v>
@@ -30343,7 +30343,7 @@
         <v>163368</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>26</v>
@@ -30377,7 +30377,7 @@
         <v>163387</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>26</v>
@@ -30411,7 +30411,7 @@
         <v>163517</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>26</v>
@@ -30445,7 +30445,7 @@
         <v>163524</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>26</v>
@@ -30479,7 +30479,7 @@
         <v>163565</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>26</v>
@@ -30513,7 +30513,7 @@
         <v>163569</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>26</v>
@@ -30547,7 +30547,7 @@
         <v>163587</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>26</v>
@@ -30581,7 +30581,7 @@
         <v>163589</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>26</v>
@@ -30615,7 +30615,7 @@
         <v>163603</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>26</v>
@@ -30649,7 +30649,7 @@
         <v>163792</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>26</v>
@@ -30683,7 +30683,7 @@
         <v>163892</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>26</v>
@@ -30717,7 +30717,7 @@
         <v>163908</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>26</v>
@@ -30751,7 +30751,7 @@
         <v>163995</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>26</v>
@@ -30785,7 +30785,7 @@
         <v>163998</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>26</v>
@@ -30819,7 +30819,7 @@
         <v>164034</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>26</v>
@@ -30853,7 +30853,7 @@
         <v>164037</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
@@ -30887,7 +30887,7 @@
         <v>164039</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
@@ -30921,7 +30921,7 @@
         <v>164041</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>26</v>
@@ -30955,7 +30955,7 @@
         <v>164043</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>26</v>
@@ -30989,7 +30989,7 @@
         <v>165679</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>26</v>
@@ -31023,7 +31023,7 @@
         <v>165877</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>26</v>
@@ -31057,7 +31057,7 @@
         <v>165878</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>26</v>
@@ -31091,7 +31091,7 @@
         <v>165993</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>26</v>
@@ -31125,7 +31125,7 @@
         <v>165998</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>26</v>
@@ -31159,7 +31159,7 @@
         <v>166365</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>26</v>
@@ -31193,7 +31193,7 @@
         <v>167229</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>26</v>
@@ -31227,7 +31227,7 @@
         <v>167233</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>26</v>
@@ -31261,7 +31261,7 @@
         <v>167234</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>26</v>
@@ -31295,7 +31295,7 @@
         <v>167680</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>26</v>
@@ -31329,7 +31329,7 @@
         <v>168093</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>26</v>
@@ -31363,7 +31363,7 @@
         <v>168130</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>26</v>
@@ -31397,7 +31397,7 @@
         <v>168132</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>26</v>
@@ -31431,7 +31431,7 @@
         <v>168139</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>26</v>
@@ -31465,7 +31465,7 @@
         <v>168141</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>26</v>
@@ -31499,7 +31499,7 @@
         <v>168144</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>26</v>
@@ -31533,7 +31533,7 @@
         <v>168154</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>26</v>
@@ -31567,7 +31567,7 @@
         <v>168158</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>26</v>
@@ -31601,7 +31601,7 @@
         <v>168160</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>26</v>
@@ -31635,7 +31635,7 @@
         <v>168161</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>26</v>
@@ -31669,7 +31669,7 @@
         <v>168163</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>26</v>
@@ -31703,7 +31703,7 @@
         <v>168165</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>26</v>
@@ -31737,7 +31737,7 @@
         <v>168166</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>26</v>
@@ -31771,7 +31771,7 @@
         <v>168167</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>26</v>
@@ -31805,7 +31805,7 @@
         <v>168175</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>26</v>
@@ -31839,7 +31839,7 @@
         <v>168487</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>26</v>
@@ -31873,7 +31873,7 @@
         <v>171882</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>26</v>
@@ -31907,7 +31907,7 @@
         <v>250</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>26</v>
@@ -31941,7 +31941,7 @@
         <v>251</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>26</v>
@@ -31975,7 +31975,7 @@
         <v>252</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>26</v>
@@ -32009,7 +32009,7 @@
         <v>253</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>26</v>
@@ -32043,7 +32043,7 @@
         <v>254</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>26</v>
@@ -32077,7 +32077,7 @@
         <v>255</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>26</v>
@@ -32111,7 +32111,7 @@
         <v>550562</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>26</v>
@@ -32145,7 +32145,7 @@
         <v>553322</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>26</v>
@@ -32179,7 +32179,7 @@
         <v>622248</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>26</v>
@@ -32213,7 +32213,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>28</v>
@@ -32247,7 +32247,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>28</v>
@@ -32281,7 +32281,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>28</v>
@@ -32315,7 +32315,7 @@
         <v>252</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>28</v>
@@ -32349,7 +32349,7 @@
         <v>251</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>28</v>
@@ -32383,7 +32383,7 @@
         <v>255</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>28</v>
@@ -32417,7 +32417,7 @@
         <v>250</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>28</v>
@@ -32451,7 +32451,7 @@
         <v>254</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>28</v>
@@ -32485,7 +32485,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>28</v>
@@ -32519,7 +32519,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>28</v>
@@ -32553,7 +32553,7 @@
         <v>253</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>28</v>
@@ -32587,7 +32587,7 @@
         <v>4</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>28</v>
@@ -32621,7 +32621,7 @@
         <v>3</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>32</v>
@@ -32655,7 +32655,7 @@
         <v>5</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>32</v>
@@ -32689,7 +32689,7 @@
         <v>6</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>32</v>
@@ -32723,7 +32723,7 @@
         <v>252</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>32</v>
@@ -32757,7 +32757,7 @@
         <v>251</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>32</v>
@@ -32791,7 +32791,7 @@
         <v>255</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>32</v>
@@ -32825,7 +32825,7 @@
         <v>250</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>32</v>
@@ -32859,7 +32859,7 @@
         <v>254</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>32</v>
@@ -32893,7 +32893,7 @@
         <v>1</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>32</v>
@@ -32927,7 +32927,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>32</v>
@@ -32961,7 +32961,7 @@
         <v>253</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>32</v>
@@ -32995,7 +32995,7 @@
         <v>4</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>32</v>
@@ -33029,7 +33029,7 @@
         <v>5</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>30</v>
@@ -33063,7 +33063,7 @@
         <v>3</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>30</v>
@@ -33097,7 +33097,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>30</v>
@@ -33131,7 +33131,7 @@
         <v>6</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>30</v>
@@ -33165,7 +33165,7 @@
         <v>4</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>30</v>
@@ -33199,7 +33199,7 @@
         <v>252</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>30</v>
@@ -33233,7 +33233,7 @@
         <v>251</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>30</v>
@@ -33267,7 +33267,7 @@
         <v>255</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>30</v>
@@ -33301,7 +33301,7 @@
         <v>1</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>30</v>
@@ -33335,7 +33335,7 @@
         <v>250</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>30</v>
@@ -33369,7 +33369,7 @@
         <v>254</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>30</v>
@@ -33403,7 +33403,7 @@
         <v>253</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>30</v>
@@ -33437,7 +33437,7 @@
         <v>5</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>34</v>
@@ -33471,7 +33471,7 @@
         <v>3</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>34</v>
@@ -33505,7 +33505,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>34</v>
@@ -33539,7 +33539,7 @@
         <v>6</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>34</v>
@@ -33573,7 +33573,7 @@
         <v>4</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>34</v>
@@ -33607,7 +33607,7 @@
         <v>252</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>34</v>
@@ -33641,7 +33641,7 @@
         <v>251</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>34</v>
@@ -33675,7 +33675,7 @@
         <v>255</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>34</v>
@@ -33709,7 +33709,7 @@
         <v>1</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>34</v>
@@ -33743,7 +33743,7 @@
         <v>250</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>34</v>
@@ -33777,7 +33777,7 @@
         <v>254</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>34</v>
@@ -33811,7 +33811,7 @@
         <v>253</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>34</v>
@@ -33845,7 +33845,7 @@
         <v>1</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>36</v>
@@ -33879,7 +33879,7 @@
         <v>3</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>36</v>
@@ -33913,7 +33913,7 @@
         <v>2</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>36</v>
@@ -33947,7 +33947,7 @@
         <v>252</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>36</v>
@@ -33981,7 +33981,7 @@
         <v>251</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>36</v>
@@ -34015,7 +34015,7 @@
         <v>255</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>36</v>
@@ -34049,7 +34049,7 @@
         <v>250</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>36</v>
@@ -34083,7 +34083,7 @@
         <v>254</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C141" s="8" t="s">
         <v>36</v>
@@ -34117,7 +34117,7 @@
         <v>253</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>36</v>
@@ -34151,7 +34151,7 @@
         <v>11</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>38</v>
@@ -34185,7 +34185,7 @@
         <v>6</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C144" s="8" t="s">
         <v>38</v>
@@ -34219,7 +34219,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C145" s="8" t="s">
         <v>38</v>
@@ -34253,7 +34253,7 @@
         <v>17</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C146" s="8" t="s">
         <v>38</v>
@@ -34287,7 +34287,7 @@
         <v>3</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C147" s="8" t="s">
         <v>38</v>
@@ -34321,7 +34321,7 @@
         <v>15</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C148" s="8" t="s">
         <v>38</v>
@@ -34355,7 +34355,7 @@
         <v>10</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C149" s="8" t="s">
         <v>38</v>
@@ -34389,7 +34389,7 @@
         <v>16</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C150" s="8" t="s">
         <v>38</v>
@@ -34423,7 +34423,7 @@
         <v>13</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>38</v>
@@ -34457,7 +34457,7 @@
         <v>14</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C152" s="8" t="s">
         <v>38</v>
@@ -34491,7 +34491,7 @@
         <v>252</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C153" s="8" t="s">
         <v>38</v>
@@ -34525,7 +34525,7 @@
         <v>251</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C154" s="8" t="s">
         <v>38</v>
@@ -34559,7 +34559,7 @@
         <v>255</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C155" s="8" t="s">
         <v>38</v>
@@ -34593,7 +34593,7 @@
         <v>250</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C156" s="8" t="s">
         <v>38</v>
@@ -34627,7 +34627,7 @@
         <v>4</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C157" s="8" t="s">
         <v>38</v>
@@ -34661,7 +34661,7 @@
         <v>7</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>38</v>
@@ -34695,7 +34695,7 @@
         <v>19</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>38</v>
@@ -34729,7 +34729,7 @@
         <v>254</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>38</v>
@@ -34763,7 +34763,7 @@
         <v>5</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>38</v>
@@ -34797,7 +34797,7 @@
         <v>8</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>38</v>
@@ -34831,7 +34831,7 @@
         <v>20</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C163" s="8" t="s">
         <v>38</v>
@@ -34865,7 +34865,7 @@
         <v>18</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C164" s="8" t="s">
         <v>38</v>
@@ -34899,7 +34899,7 @@
         <v>253</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C165" s="8" t="s">
         <v>38</v>
@@ -34933,7 +34933,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>38</v>
@@ -34967,7 +34967,7 @@
         <v>1</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C167" s="8" t="s">
         <v>38</v>
@@ -35001,7 +35001,7 @@
         <v>2</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C168" s="8" t="s">
         <v>38</v>
@@ -35035,7 +35035,7 @@
         <v>2</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C169" s="8" t="s">
         <v>56</v>
@@ -35069,7 +35069,7 @@
         <v>252</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>56</v>
@@ -35103,7 +35103,7 @@
         <v>251</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>56</v>
@@ -35137,7 +35137,7 @@
         <v>255</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>56</v>
@@ -35171,7 +35171,7 @@
         <v>250</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C173" s="8" t="s">
         <v>56</v>
@@ -35205,7 +35205,7 @@
         <v>254</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C174" s="8" t="s">
         <v>56</v>
@@ -35239,7 +35239,7 @@
         <v>253</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>56</v>
@@ -35273,7 +35273,7 @@
         <v>1</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C176" s="8" t="s">
         <v>56</v>
@@ -35307,7 +35307,7 @@
         <v>2</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C177" s="8" t="s">
         <v>52</v>
@@ -35341,7 +35341,7 @@
         <v>252</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C178" s="8" t="s">
         <v>52</v>
@@ -35375,7 +35375,7 @@
         <v>251</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C179" s="8" t="s">
         <v>52</v>
@@ -35409,7 +35409,7 @@
         <v>255</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C180" s="8" t="s">
         <v>52</v>
@@ -35443,7 +35443,7 @@
         <v>250</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C181" s="8" t="s">
         <v>52</v>
@@ -35477,7 +35477,7 @@
         <v>254</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C182" s="8" t="s">
         <v>52</v>
@@ -35511,7 +35511,7 @@
         <v>253</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C183" s="8" t="s">
         <v>52</v>
@@ -35545,7 +35545,7 @@
         <v>1</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C184" s="8" t="s">
         <v>52</v>
@@ -35579,7 +35579,7 @@
         <v>2</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C185" s="8" t="s">
         <v>54</v>
@@ -35613,7 +35613,7 @@
         <v>252</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C186" s="8" t="s">
         <v>54</v>
@@ -35647,7 +35647,7 @@
         <v>251</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C187" s="8" t="s">
         <v>54</v>
@@ -35681,7 +35681,7 @@
         <v>255</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C188" s="8" t="s">
         <v>54</v>
@@ -35715,7 +35715,7 @@
         <v>250</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C189" s="8" t="s">
         <v>54</v>
@@ -35749,7 +35749,7 @@
         <v>254</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C190" s="8" t="s">
         <v>54</v>
@@ -35783,7 +35783,7 @@
         <v>253</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C191" s="8" t="s">
         <v>54</v>
@@ -35817,7 +35817,7 @@
         <v>1</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C192" s="8" t="s">
         <v>54</v>
@@ -35851,7 +35851,7 @@
         <v>2</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>64</v>
@@ -35885,7 +35885,7 @@
         <v>5</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>64</v>
@@ -35919,7 +35919,7 @@
         <v>4</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>64</v>
@@ -35953,7 +35953,7 @@
         <v>252</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C196" s="9" t="s">
         <v>64</v>
@@ -35987,7 +35987,7 @@
         <v>251</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C197" s="9" t="s">
         <v>64</v>
@@ -36021,7 +36021,7 @@
         <v>255</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>64</v>
@@ -36055,7 +36055,7 @@
         <v>250</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>64</v>
@@ -36089,7 +36089,7 @@
         <v>254</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C200" s="9" t="s">
         <v>64</v>
@@ -36123,7 +36123,7 @@
         <v>6</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C201" s="9" t="s">
         <v>64</v>
@@ -36157,7 +36157,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>64</v>
@@ -36191,7 +36191,7 @@
         <v>253</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C203" s="9" t="s">
         <v>64</v>
@@ -36225,7 +36225,7 @@
         <v>3</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>64</v>
@@ -36259,7 +36259,7 @@
         <v>3000</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>66</v>
@@ -36293,7 +36293,7 @@
         <v>44000</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>66</v>
@@ -36327,7 +36327,7 @@
         <v>52000</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>66</v>
@@ -36361,7 +36361,7 @@
         <v>51000</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C208" s="9" t="s">
         <v>66</v>
@@ -36395,7 +36395,7 @@
         <v>5000</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>66</v>
@@ -36429,7 +36429,7 @@
         <v>46000</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>66</v>
@@ -36463,7 +36463,7 @@
         <v>4000</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>66</v>
@@ -36497,7 +36497,7 @@
         <v>45000</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C212" s="9" t="s">
         <v>66</v>
@@ -36531,7 +36531,7 @@
         <v>252</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C213" s="9" t="s">
         <v>66</v>
@@ -36565,7 +36565,7 @@
         <v>251</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>66</v>
@@ -36599,7 +36599,7 @@
         <v>255</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C215" s="9" t="s">
         <v>66</v>
@@ -36633,7 +36633,7 @@
         <v>53000</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C216" s="9" t="s">
         <v>66</v>
@@ -36667,7 +36667,7 @@
         <v>54000</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C217" s="9" t="s">
         <v>66</v>
@@ -36701,7 +36701,7 @@
         <v>55000</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C218" s="9" t="s">
         <v>66</v>
@@ -36735,7 +36735,7 @@
         <v>56000</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C219" s="9" t="s">
         <v>66</v>
@@ -36769,7 +36769,7 @@
         <v>50000</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C220" s="9" t="s">
         <v>66</v>
@@ -36803,7 +36803,7 @@
         <v>7000</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C221" s="9" t="s">
         <v>66</v>
@@ -36837,7 +36837,7 @@
         <v>2000</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C222" s="9" t="s">
         <v>66</v>
@@ -36871,7 +36871,7 @@
         <v>43000</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C223" s="9" t="s">
         <v>66</v>
@@ -36905,7 +36905,7 @@
         <v>6000</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C224" s="9" t="s">
         <v>66</v>
@@ -36939,7 +36939,7 @@
         <v>47000</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C225" s="9" t="s">
         <v>66</v>
@@ -36973,7 +36973,7 @@
         <v>90000</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C226" s="9" t="s">
         <v>66</v>
@@ -37007,7 +37007,7 @@
         <v>253</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C227" s="9" t="s">
         <v>66</v>
@@ -37041,7 +37041,7 @@
         <v>2001</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C228" s="9" t="s">
         <v>68</v>
@@ -37075,7 +37075,7 @@
         <v>44018</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C229" s="9" t="s">
         <v>68</v>
@@ -37109,7 +37109,7 @@
         <v>44007</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>68</v>
@@ -37143,7 +37143,7 @@
         <v>44017</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C231" s="9" t="s">
         <v>68</v>
@@ -37177,7 +37177,7 @@
         <v>44016</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>68</v>
@@ -37211,7 +37211,7 @@
         <v>44013</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C233" s="9" t="s">
         <v>68</v>
@@ -37245,7 +37245,7 @@
         <v>3001</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C234" s="9" t="s">
         <v>68</v>
@@ -37279,7 +37279,7 @@
         <v>3002</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C235" s="9" t="s">
         <v>68</v>
@@ -37313,7 +37313,7 @@
         <v>52003</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C236" s="9" t="s">
         <v>68</v>
@@ -37347,7 +37347,7 @@
         <v>51002</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C237" s="9" t="s">
         <v>68</v>
@@ -37381,7 +37381,7 @@
         <v>51003</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C238" s="9" t="s">
         <v>68</v>
@@ -37415,7 +37415,7 @@
         <v>52001</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C239" s="9" t="s">
         <v>68</v>
@@ -37449,7 +37449,7 @@
         <v>52002</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C240" s="9" t="s">
         <v>68</v>
@@ -37483,7 +37483,7 @@
         <v>52004</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>68</v>
@@ -37517,7 +37517,7 @@
         <v>90001</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>68</v>
@@ -37551,7 +37551,7 @@
         <v>46003</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>68</v>
@@ -37585,7 +37585,7 @@
         <v>46001</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C244" s="9" t="s">
         <v>68</v>
@@ -37619,7 +37619,7 @@
         <v>46004</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C245" s="9" t="s">
         <v>68</v>
@@ -37653,7 +37653,7 @@
         <v>5001</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C246" s="9" t="s">
         <v>68</v>
@@ -37687,7 +37687,7 @@
         <v>5003</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C247" s="9" t="s">
         <v>68</v>
@@ -37721,7 +37721,7 @@
         <v>5002</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C248" s="9" t="s">
         <v>68</v>
@@ -37755,7 +37755,7 @@
         <v>4001</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C249" s="9" t="s">
         <v>68</v>
@@ -37789,7 +37789,7 @@
         <v>4002</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C250" s="9" t="s">
         <v>68</v>
@@ -37823,7 +37823,7 @@
         <v>44010</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C251" s="9" t="s">
         <v>68</v>
@@ -37857,7 +37857,7 @@
         <v>51001</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C252" s="9" t="s">
         <v>68</v>
@@ -37891,7 +37891,7 @@
         <v>46002</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C253" s="9" t="s">
         <v>68</v>
@@ -37925,7 +37925,7 @@
         <v>43000</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C254" s="9" t="s">
         <v>68</v>
@@ -37959,7 +37959,7 @@
         <v>44000</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C255" s="9" t="s">
         <v>68</v>
@@ -37993,7 +37993,7 @@
         <v>45000</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C256" s="9" t="s">
         <v>68</v>
@@ -38027,7 +38027,7 @@
         <v>46000</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C257" s="9" t="s">
         <v>68</v>
@@ -38061,7 +38061,7 @@
         <v>47000</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C258" s="9" t="s">
         <v>68</v>
@@ -38095,7 +38095,7 @@
         <v>50000</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C259" s="9" t="s">
         <v>68</v>
@@ -38129,7 +38129,7 @@
         <v>51000</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>68</v>
@@ -38163,7 +38163,7 @@
         <v>52000</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>68</v>
@@ -38197,7 +38197,7 @@
         <v>53000</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>68</v>
@@ -38231,7 +38231,7 @@
         <v>54000</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>68</v>
@@ -38265,7 +38265,7 @@
         <v>55000</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>68</v>
@@ -38299,7 +38299,7 @@
         <v>56000</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>68</v>
@@ -38333,7 +38333,7 @@
         <v>90000</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>68</v>
@@ -38367,7 +38367,7 @@
         <v>44001</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>68</v>
@@ -38401,7 +38401,7 @@
         <v>44003</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>68</v>
@@ -38435,7 +38435,7 @@
         <v>44002</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>68</v>
@@ -38469,7 +38469,7 @@
         <v>44004</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>68</v>
@@ -38503,7 +38503,7 @@
         <v>47002</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>68</v>
@@ -38537,7 +38537,7 @@
         <v>47001</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>68</v>
@@ -38571,7 +38571,7 @@
         <v>44009</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>68</v>
@@ -38605,7 +38605,7 @@
         <v>44006</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>68</v>
@@ -38639,7 +38639,7 @@
         <v>44008</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>68</v>
@@ -38673,7 +38673,7 @@
         <v>7002</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>68</v>
@@ -38707,7 +38707,7 @@
         <v>7003</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>68</v>
@@ -38741,7 +38741,7 @@
         <v>44012</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>68</v>
@@ -38775,7 +38775,7 @@
         <v>44014</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>68</v>
@@ -38809,7 +38809,7 @@
         <v>44011</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>68</v>
@@ -38843,7 +38843,7 @@
         <v>44015</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>68</v>
@@ -38877,7 +38877,7 @@
         <v>44005</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>68</v>
@@ -38911,7 +38911,7 @@
         <v>43001</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C283" s="9" t="s">
         <v>68</v>
@@ -38945,7 +38945,7 @@
         <v>2004</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>68</v>
@@ -38979,7 +38979,7 @@
         <v>2003</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C285" s="9" t="s">
         <v>68</v>
@@ -39013,7 +39013,7 @@
         <v>2002</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C286" s="9" t="s">
         <v>68</v>
@@ -39047,7 +39047,7 @@
         <v>2005</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>68</v>
@@ -39081,7 +39081,7 @@
         <v>6002</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>68</v>
@@ -39115,7 +39115,7 @@
         <v>6003</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C289" s="9" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
fixes enumeration issues and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_catch_metadata.xlsx
+++ b/data-raw/metadata/camp_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A120872E-8722-3D42-8128-0037FE205CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA58B6B5-A7DB-034A-9694-1042AC83A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="151">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -106,9 +106,6 @@
     <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
-    <t>finalRunID</t>
-  </si>
-  <si>
     <t>Code for origin/production type of the fish.</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
     <t>Date and time of day associated with the trap visit. Definition varies based on visitType (For visitTypeID=1, 2, or 3 this is the date and the time of day the trap began fishing. For visitTypeID=4, 5, or 6 this is the date and the time of day of the end of the visit.)</t>
   </si>
   <si>
-    <t>visitTypeID</t>
-  </si>
-  <si>
-    <t>Code for work that was done during visit to trap</t>
-  </si>
-  <si>
     <t>siteID</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Not recorded</t>
   </si>
   <si>
@@ -205,28 +193,7 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>See Comments</t>
-  </si>
-  <si>
     <t>Not yet assigned</t>
-  </si>
-  <si>
-    <t>Continue trapping</t>
-  </si>
-  <si>
-    <t>Drive-by only</t>
-  </si>
-  <si>
-    <t>End trapping</t>
-  </si>
-  <si>
-    <t>Service/adjust/clean trap</t>
-  </si>
-  <si>
-    <t>Start trap &amp; begin trapping</t>
-  </si>
-  <si>
-    <t>Unplanned restart</t>
   </si>
   <si>
     <t>Eye Riffle</t>
@@ -509,6 +476,17 @@
   </si>
   <si>
     <t>Code for whether the count (n) is an actual count or estimate. Levels = c("No", "Yes")</t>
+  </si>
+  <si>
+    <t>visitType</t>
+  </si>
+  <si>
+    <t>Code for work that was done during visit to trap. Levels = c("Continue trapping", "End trapping", "Start trap &amp; begin trapping", 
+"Unplanned restart", "Service/adjust/clean trap", "Drive-by only"
+)</t>
+  </si>
+  <si>
+    <t>finalRun</t>
   </si>
 </sst>
 </file>
@@ -830,9 +808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1023,28 +1001,28 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
@@ -1071,28 +1049,28 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
@@ -1119,28 +1097,28 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
@@ -1167,28 +1145,28 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
@@ -1253,33 +1231,33 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1297,33 +1275,33 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="11" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1341,10 +1319,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -1353,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1379,10 +1357,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1417,10 +1395,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1455,10 +1433,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1493,10 +1471,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
@@ -1531,10 +1509,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -1569,10 +1547,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1607,10 +1585,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1645,10 +1623,10 @@
     </row>
     <row r="20" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -1683,10 +1661,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -1721,10 +1699,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
@@ -1759,10 +1737,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
@@ -28641,10 +28619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z810"/>
+  <dimension ref="A1:Z798"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28657,13 +28635,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28694,7 +28672,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>13</v>
@@ -28725,13 +28703,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
-        <v>2</v>
+        <v>3000</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -28759,13 +28737,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
-        <v>5</v>
+        <v>44000</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -28793,13 +28771,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
-        <v>4</v>
+        <v>52000</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -28827,13 +28805,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
-        <v>252</v>
+        <v>51000</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -28861,13 +28839,13 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
-        <v>251</v>
+        <v>5000</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -28895,13 +28873,13 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
-        <v>255</v>
+        <v>46000</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -28929,13 +28907,13 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
-        <v>250</v>
+        <v>4000</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -28963,13 +28941,13 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
-        <v>254</v>
+        <v>45000</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -28997,13 +28975,13 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -29031,13 +29009,13 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -29065,13 +29043,13 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -29099,13 +29077,13 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
-        <v>3</v>
+        <v>53000</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -29133,13 +29111,13 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
-        <v>3000</v>
+        <v>54000</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -29167,13 +29145,13 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
-        <v>44000</v>
+        <v>55000</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -29201,13 +29179,13 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
-        <v>52000</v>
+        <v>56000</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -29235,13 +29213,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
-        <v>51000</v>
+        <v>50000</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -29269,13 +29247,13 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -29303,13 +29281,13 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
-        <v>46000</v>
+        <v>2000</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -29337,13 +29315,13 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
-        <v>4000</v>
+        <v>43000</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -29371,13 +29349,13 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
-        <v>45000</v>
+        <v>6000</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -29405,13 +29383,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
-        <v>252</v>
+        <v>47000</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -29439,13 +29417,13 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
-        <v>251</v>
+        <v>90000</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -29473,13 +29451,13 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -29507,13 +29485,13 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
-        <v>53000</v>
+        <v>2001</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -29541,13 +29519,13 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
-        <v>54000</v>
+        <v>44018</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -29575,13 +29553,13 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
-        <v>55000</v>
+        <v>44007</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -29609,13 +29587,13 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <v>56000</v>
+        <v>44017</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -29643,13 +29621,13 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
-        <v>50000</v>
+        <v>44016</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -29677,13 +29655,13 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
-        <v>7000</v>
+        <v>44013</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -29711,13 +29689,13 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
-        <v>2000</v>
+        <v>3001</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>82</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -29745,13 +29723,13 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
-        <v>43000</v>
+        <v>3002</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>83</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -29779,13 +29757,13 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
-        <v>6000</v>
+        <v>52003</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -29813,13 +29791,13 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
-        <v>47000</v>
+        <v>51002</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>85</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -29847,13 +29825,13 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
-        <v>90000</v>
+        <v>51003</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -29881,13 +29859,13 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
-        <v>253</v>
+        <v>52001</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -29915,13 +29893,13 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
-        <v>2001</v>
+        <v>52002</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -29949,13 +29927,13 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
-        <v>44018</v>
+        <v>52004</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -29983,13 +29961,13 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
-        <v>44007</v>
+        <v>90001</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -30017,13 +29995,13 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
-        <v>44017</v>
+        <v>46003</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -30051,13 +30029,13 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
-        <v>44016</v>
+        <v>46001</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -30085,13 +30063,13 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
-        <v>44013</v>
+        <v>46004</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -30119,13 +30097,13 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
-        <v>3001</v>
+        <v>5001</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -30153,13 +30131,13 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
-        <v>3002</v>
+        <v>5003</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -30187,13 +30165,13 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
-        <v>52003</v>
+        <v>5002</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -30221,13 +30199,13 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
-        <v>51002</v>
+        <v>4001</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -30255,13 +30233,13 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
-        <v>51003</v>
+        <v>4002</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -30289,13 +30267,13 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
-        <v>52001</v>
+        <v>44010</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>98</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -30323,13 +30301,13 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
-        <v>52002</v>
+        <v>51001</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -30357,13 +30335,13 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
-        <v>52004</v>
+        <v>46002</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>100</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -30391,13 +30369,13 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
-        <v>90001</v>
+        <v>43000</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -30425,13 +30403,13 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
-        <v>46003</v>
+        <v>44000</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -30459,13 +30437,13 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
-        <v>46001</v>
+        <v>45000</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -30493,13 +30471,13 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
-        <v>46004</v>
+        <v>46000</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -30527,13 +30505,13 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
-        <v>5001</v>
+        <v>47000</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
@@ -30561,13 +30539,13 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
-        <v>5003</v>
+        <v>50000</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -30595,13 +30573,13 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
-        <v>5002</v>
+        <v>51000</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -30629,13 +30607,13 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
-        <v>4001</v>
+        <v>52000</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -30663,13 +30641,13 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
-        <v>4002</v>
+        <v>53000</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -30697,13 +30675,13 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
-        <v>44010</v>
+        <v>54000</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -30731,13 +30709,13 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
-        <v>51001</v>
+        <v>55000</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -30765,13 +30743,13 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
-        <v>46002</v>
+        <v>56000</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
@@ -30799,13 +30777,13 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
-        <v>43000</v>
+        <v>90000</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -30833,13 +30811,13 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -30867,13 +30845,13 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9">
-        <v>45000</v>
+        <v>44003</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -30901,13 +30879,13 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
-        <v>46000</v>
+        <v>44002</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -30935,13 +30913,13 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="9">
-        <v>47000</v>
+        <v>44004</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -30969,13 +30947,13 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
-        <v>50000</v>
+        <v>47002</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -31003,13 +30981,13 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
-        <v>51000</v>
+        <v>47001</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -31037,13 +31015,13 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
-        <v>52000</v>
+        <v>44009</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -31071,13 +31049,13 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9">
-        <v>53000</v>
+        <v>44006</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -31105,13 +31083,13 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
-        <v>54000</v>
+        <v>44008</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -31139,13 +31117,13 @@
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
-        <v>55000</v>
+        <v>7002</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -31173,13 +31151,13 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9">
-        <v>56000</v>
+        <v>7003</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -31207,13 +31185,13 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
-        <v>90000</v>
+        <v>44012</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -31241,13 +31219,13 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9">
-        <v>44001</v>
+        <v>44014</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -31275,13 +31253,13 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
-        <v>44003</v>
+        <v>44011</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -31309,13 +31287,13 @@
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
-        <v>44002</v>
+        <v>44015</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -31343,13 +31321,13 @@
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9">
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -31377,13 +31355,13 @@
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
-        <v>47002</v>
+        <v>43001</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -31411,13 +31389,13 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
-        <v>47001</v>
+        <v>2004</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
@@ -31445,13 +31423,13 @@
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9">
-        <v>44009</v>
+        <v>2003</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
@@ -31479,13 +31457,13 @@
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
-        <v>44006</v>
+        <v>2002</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -31513,13 +31491,13 @@
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
-        <v>44008</v>
+        <v>2005</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -31547,13 +31525,13 @@
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
-        <v>7002</v>
+        <v>6002</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -31581,13 +31559,13 @@
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
-        <v>7003</v>
+        <v>6003</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -31614,15 +31592,9 @@
       <c r="Z87" s="9"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="9">
-        <v>44012</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
@@ -31648,15 +31620,9 @@
       <c r="Z88" s="9"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="9">
-        <v>44014</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -31682,15 +31648,9 @@
       <c r="Z89" s="9"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="9">
-        <v>44011</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -31716,15 +31676,9 @@
       <c r="Z90" s="9"/>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="9">
-        <v>44015</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
@@ -31750,15 +31704,9 @@
       <c r="Z91" s="9"/>
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="9">
-        <v>44005</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
@@ -31784,15 +31732,9 @@
       <c r="Z92" s="9"/>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="9">
-        <v>43001</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
@@ -31818,15 +31760,9 @@
       <c r="Z93" s="9"/>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="9">
-        <v>2004</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
@@ -31852,15 +31788,9 @@
       <c r="Z94" s="9"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="9">
-        <v>2003</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
@@ -31886,15 +31816,9 @@
       <c r="Z95" s="9"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="9">
-        <v>2002</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
@@ -31920,15 +31844,9 @@
       <c r="Z96" s="9"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="9">
-        <v>2005</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
@@ -31954,15 +31872,9 @@
       <c r="Z97" s="9"/>
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="9">
-        <v>6002</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
@@ -31988,15 +31900,9 @@
       <c r="Z98" s="9"/>
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="9">
-        <v>6003</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
@@ -51593,342 +51499,6 @@
       <c r="Y798" s="9"/>
       <c r="Z798" s="9"/>
     </row>
-    <row r="799" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A799" s="8"/>
-      <c r="B799" s="8"/>
-      <c r="C799" s="8"/>
-      <c r="D799" s="9"/>
-      <c r="E799" s="9"/>
-      <c r="F799" s="9"/>
-      <c r="G799" s="9"/>
-      <c r="H799" s="9"/>
-      <c r="I799" s="9"/>
-      <c r="J799" s="9"/>
-      <c r="K799" s="9"/>
-      <c r="L799" s="9"/>
-      <c r="M799" s="9"/>
-      <c r="N799" s="9"/>
-      <c r="O799" s="9"/>
-      <c r="P799" s="9"/>
-      <c r="Q799" s="9"/>
-      <c r="R799" s="9"/>
-      <c r="S799" s="9"/>
-      <c r="T799" s="9"/>
-      <c r="U799" s="9"/>
-      <c r="V799" s="9"/>
-      <c r="W799" s="9"/>
-      <c r="X799" s="9"/>
-      <c r="Y799" s="9"/>
-      <c r="Z799" s="9"/>
-    </row>
-    <row r="800" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A800" s="8"/>
-      <c r="B800" s="8"/>
-      <c r="C800" s="8"/>
-      <c r="D800" s="9"/>
-      <c r="E800" s="9"/>
-      <c r="F800" s="9"/>
-      <c r="G800" s="9"/>
-      <c r="H800" s="9"/>
-      <c r="I800" s="9"/>
-      <c r="J800" s="9"/>
-      <c r="K800" s="9"/>
-      <c r="L800" s="9"/>
-      <c r="M800" s="9"/>
-      <c r="N800" s="9"/>
-      <c r="O800" s="9"/>
-      <c r="P800" s="9"/>
-      <c r="Q800" s="9"/>
-      <c r="R800" s="9"/>
-      <c r="S800" s="9"/>
-      <c r="T800" s="9"/>
-      <c r="U800" s="9"/>
-      <c r="V800" s="9"/>
-      <c r="W800" s="9"/>
-      <c r="X800" s="9"/>
-      <c r="Y800" s="9"/>
-      <c r="Z800" s="9"/>
-    </row>
-    <row r="801" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A801" s="8"/>
-      <c r="B801" s="8"/>
-      <c r="C801" s="8"/>
-      <c r="D801" s="9"/>
-      <c r="E801" s="9"/>
-      <c r="F801" s="9"/>
-      <c r="G801" s="9"/>
-      <c r="H801" s="9"/>
-      <c r="I801" s="9"/>
-      <c r="J801" s="9"/>
-      <c r="K801" s="9"/>
-      <c r="L801" s="9"/>
-      <c r="M801" s="9"/>
-      <c r="N801" s="9"/>
-      <c r="O801" s="9"/>
-      <c r="P801" s="9"/>
-      <c r="Q801" s="9"/>
-      <c r="R801" s="9"/>
-      <c r="S801" s="9"/>
-      <c r="T801" s="9"/>
-      <c r="U801" s="9"/>
-      <c r="V801" s="9"/>
-      <c r="W801" s="9"/>
-      <c r="X801" s="9"/>
-      <c r="Y801" s="9"/>
-      <c r="Z801" s="9"/>
-    </row>
-    <row r="802" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A802" s="8"/>
-      <c r="B802" s="8"/>
-      <c r="C802" s="8"/>
-      <c r="D802" s="9"/>
-      <c r="E802" s="9"/>
-      <c r="F802" s="9"/>
-      <c r="G802" s="9"/>
-      <c r="H802" s="9"/>
-      <c r="I802" s="9"/>
-      <c r="J802" s="9"/>
-      <c r="K802" s="9"/>
-      <c r="L802" s="9"/>
-      <c r="M802" s="9"/>
-      <c r="N802" s="9"/>
-      <c r="O802" s="9"/>
-      <c r="P802" s="9"/>
-      <c r="Q802" s="9"/>
-      <c r="R802" s="9"/>
-      <c r="S802" s="9"/>
-      <c r="T802" s="9"/>
-      <c r="U802" s="9"/>
-      <c r="V802" s="9"/>
-      <c r="W802" s="9"/>
-      <c r="X802" s="9"/>
-      <c r="Y802" s="9"/>
-      <c r="Z802" s="9"/>
-    </row>
-    <row r="803" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A803" s="8"/>
-      <c r="B803" s="8"/>
-      <c r="C803" s="8"/>
-      <c r="D803" s="9"/>
-      <c r="E803" s="9"/>
-      <c r="F803" s="9"/>
-      <c r="G803" s="9"/>
-      <c r="H803" s="9"/>
-      <c r="I803" s="9"/>
-      <c r="J803" s="9"/>
-      <c r="K803" s="9"/>
-      <c r="L803" s="9"/>
-      <c r="M803" s="9"/>
-      <c r="N803" s="9"/>
-      <c r="O803" s="9"/>
-      <c r="P803" s="9"/>
-      <c r="Q803" s="9"/>
-      <c r="R803" s="9"/>
-      <c r="S803" s="9"/>
-      <c r="T803" s="9"/>
-      <c r="U803" s="9"/>
-      <c r="V803" s="9"/>
-      <c r="W803" s="9"/>
-      <c r="X803" s="9"/>
-      <c r="Y803" s="9"/>
-      <c r="Z803" s="9"/>
-    </row>
-    <row r="804" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A804" s="8"/>
-      <c r="B804" s="8"/>
-      <c r="C804" s="8"/>
-      <c r="D804" s="9"/>
-      <c r="E804" s="9"/>
-      <c r="F804" s="9"/>
-      <c r="G804" s="9"/>
-      <c r="H804" s="9"/>
-      <c r="I804" s="9"/>
-      <c r="J804" s="9"/>
-      <c r="K804" s="9"/>
-      <c r="L804" s="9"/>
-      <c r="M804" s="9"/>
-      <c r="N804" s="9"/>
-      <c r="O804" s="9"/>
-      <c r="P804" s="9"/>
-      <c r="Q804" s="9"/>
-      <c r="R804" s="9"/>
-      <c r="S804" s="9"/>
-      <c r="T804" s="9"/>
-      <c r="U804" s="9"/>
-      <c r="V804" s="9"/>
-      <c r="W804" s="9"/>
-      <c r="X804" s="9"/>
-      <c r="Y804" s="9"/>
-      <c r="Z804" s="9"/>
-    </row>
-    <row r="805" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A805" s="8"/>
-      <c r="B805" s="8"/>
-      <c r="C805" s="8"/>
-      <c r="D805" s="9"/>
-      <c r="E805" s="9"/>
-      <c r="F805" s="9"/>
-      <c r="G805" s="9"/>
-      <c r="H805" s="9"/>
-      <c r="I805" s="9"/>
-      <c r="J805" s="9"/>
-      <c r="K805" s="9"/>
-      <c r="L805" s="9"/>
-      <c r="M805" s="9"/>
-      <c r="N805" s="9"/>
-      <c r="O805" s="9"/>
-      <c r="P805" s="9"/>
-      <c r="Q805" s="9"/>
-      <c r="R805" s="9"/>
-      <c r="S805" s="9"/>
-      <c r="T805" s="9"/>
-      <c r="U805" s="9"/>
-      <c r="V805" s="9"/>
-      <c r="W805" s="9"/>
-      <c r="X805" s="9"/>
-      <c r="Y805" s="9"/>
-      <c r="Z805" s="9"/>
-    </row>
-    <row r="806" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A806" s="8"/>
-      <c r="B806" s="8"/>
-      <c r="C806" s="8"/>
-      <c r="D806" s="9"/>
-      <c r="E806" s="9"/>
-      <c r="F806" s="9"/>
-      <c r="G806" s="9"/>
-      <c r="H806" s="9"/>
-      <c r="I806" s="9"/>
-      <c r="J806" s="9"/>
-      <c r="K806" s="9"/>
-      <c r="L806" s="9"/>
-      <c r="M806" s="9"/>
-      <c r="N806" s="9"/>
-      <c r="O806" s="9"/>
-      <c r="P806" s="9"/>
-      <c r="Q806" s="9"/>
-      <c r="R806" s="9"/>
-      <c r="S806" s="9"/>
-      <c r="T806" s="9"/>
-      <c r="U806" s="9"/>
-      <c r="V806" s="9"/>
-      <c r="W806" s="9"/>
-      <c r="X806" s="9"/>
-      <c r="Y806" s="9"/>
-      <c r="Z806" s="9"/>
-    </row>
-    <row r="807" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A807" s="8"/>
-      <c r="B807" s="8"/>
-      <c r="C807" s="8"/>
-      <c r="D807" s="9"/>
-      <c r="E807" s="9"/>
-      <c r="F807" s="9"/>
-      <c r="G807" s="9"/>
-      <c r="H807" s="9"/>
-      <c r="I807" s="9"/>
-      <c r="J807" s="9"/>
-      <c r="K807" s="9"/>
-      <c r="L807" s="9"/>
-      <c r="M807" s="9"/>
-      <c r="N807" s="9"/>
-      <c r="O807" s="9"/>
-      <c r="P807" s="9"/>
-      <c r="Q807" s="9"/>
-      <c r="R807" s="9"/>
-      <c r="S807" s="9"/>
-      <c r="T807" s="9"/>
-      <c r="U807" s="9"/>
-      <c r="V807" s="9"/>
-      <c r="W807" s="9"/>
-      <c r="X807" s="9"/>
-      <c r="Y807" s="9"/>
-      <c r="Z807" s="9"/>
-    </row>
-    <row r="808" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A808" s="8"/>
-      <c r="B808" s="8"/>
-      <c r="C808" s="8"/>
-      <c r="D808" s="9"/>
-      <c r="E808" s="9"/>
-      <c r="F808" s="9"/>
-      <c r="G808" s="9"/>
-      <c r="H808" s="9"/>
-      <c r="I808" s="9"/>
-      <c r="J808" s="9"/>
-      <c r="K808" s="9"/>
-      <c r="L808" s="9"/>
-      <c r="M808" s="9"/>
-      <c r="N808" s="9"/>
-      <c r="O808" s="9"/>
-      <c r="P808" s="9"/>
-      <c r="Q808" s="9"/>
-      <c r="R808" s="9"/>
-      <c r="S808" s="9"/>
-      <c r="T808" s="9"/>
-      <c r="U808" s="9"/>
-      <c r="V808" s="9"/>
-      <c r="W808" s="9"/>
-      <c r="X808" s="9"/>
-      <c r="Y808" s="9"/>
-      <c r="Z808" s="9"/>
-    </row>
-    <row r="809" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A809" s="8"/>
-      <c r="B809" s="8"/>
-      <c r="C809" s="8"/>
-      <c r="D809" s="9"/>
-      <c r="E809" s="9"/>
-      <c r="F809" s="9"/>
-      <c r="G809" s="9"/>
-      <c r="H809" s="9"/>
-      <c r="I809" s="9"/>
-      <c r="J809" s="9"/>
-      <c r="K809" s="9"/>
-      <c r="L809" s="9"/>
-      <c r="M809" s="9"/>
-      <c r="N809" s="9"/>
-      <c r="O809" s="9"/>
-      <c r="P809" s="9"/>
-      <c r="Q809" s="9"/>
-      <c r="R809" s="9"/>
-      <c r="S809" s="9"/>
-      <c r="T809" s="9"/>
-      <c r="U809" s="9"/>
-      <c r="V809" s="9"/>
-      <c r="W809" s="9"/>
-      <c r="X809" s="9"/>
-      <c r="Y809" s="9"/>
-      <c r="Z809" s="9"/>
-    </row>
-    <row r="810" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A810" s="8"/>
-      <c r="B810" s="8"/>
-      <c r="C810" s="8"/>
-      <c r="D810" s="9"/>
-      <c r="E810" s="9"/>
-      <c r="F810" s="9"/>
-      <c r="G810" s="9"/>
-      <c r="H810" s="9"/>
-      <c r="I810" s="9"/>
-      <c r="J810" s="9"/>
-      <c r="K810" s="9"/>
-      <c r="L810" s="9"/>
-      <c r="M810" s="9"/>
-      <c r="N810" s="9"/>
-      <c r="O810" s="9"/>
-      <c r="P810" s="9"/>
-      <c r="Q810" s="9"/>
-      <c r="R810" s="9"/>
-      <c r="S810" s="9"/>
-      <c r="T810" s="9"/>
-      <c r="U810" s="9"/>
-      <c r="V810" s="9"/>
-      <c r="W810" s="9"/>
-      <c r="X810" s="9"/>
-      <c r="Y810" s="9"/>
-      <c r="Z810" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>